<commit_message>
Adding new project and recent changes to Powershell project
</commit_message>
<xml_diff>
--- a/Equipment_Registration_App/Equipment_Registration_App/Minuta_computadores.xlsx
+++ b/Equipment_Registration_App/Equipment_Registration_App/Minuta_computadores.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andresfelipe.perez\PycharmProjects\Equipment_Registration_App\Equipment_Registration_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA4832A-F461-417C-B583-C0B8FA6C57E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BCE9B4-4F31-42FB-9EC2-F38A7BDAFDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="148YiuHQ5lXJWUToTkvr1pwXzj+ON8cfZP+R9+O7wvSWExp7uaLSY8+ZU4BF1xL+EAgdMPlgOXlUkIOTH75cUA==" workbookSaltValue="r//egdUdAhMm1PxcbXxveQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{25B8F748-A59F-4FB4-B0F7-CE2AC7157BE1}"/>
+    <workbookView xWindow="-14460" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{25B8F748-A59F-4FB4-B0F7-CE2AC7157BE1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Minuta de registro" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Minuta de registro'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -106,11 +107,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,17 +432,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="29.21875" customWidth="1"/>
     <col min="4" max="4" width="22.21875" customWidth="1"/>
     <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" customWidth="1"/>
     <col min="8" max="8" width="20.44140625" customWidth="1"/>
     <col min="9" max="10" width="22.44140625" customWidth="1"/>
@@ -447,10 +450,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -462,7 +465,7 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -482,8 +485,10 @@
       <c r="M1" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="RiV79UDehaDkj8Ifbx3VOBdPAwOFkI32t3/LVbTYrRsQrYijRwkZaM889Og7+1hOCfUtDZsKa4hBBBIuTPkyPw==" saltValue="q7PUUS1EfTvFDCV1LviGMw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A1:J1" xr:uid="{F6B7ACFC-1D68-4C1C-85DA-B914FE1B0D40}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K737373 Asurion_Internal_Use_Only</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Powershell App Final Version
</commit_message>
<xml_diff>
--- a/Equipment_Registration_App/Equipment_Registration_App/Minuta_computadores.xlsx
+++ b/Equipment_Registration_App/Equipment_Registration_App/Minuta_computadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andresfelipe.perez\PycharmProjects\Equipment_Registration_App\Equipment_Registration_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BCE9B4-4F31-42FB-9EC2-F38A7BDAFDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429E190F-D113-47AE-912F-EAD482528061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="148YiuHQ5lXJWUToTkvr1pwXzj+ON8cfZP+R9+O7wvSWExp7uaLSY8+ZU4BF1xL+EAgdMPlgOXlUkIOTH75cUA==" workbookSaltValue="r//egdUdAhMm1PxcbXxveQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-14460" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{25B8F748-A59F-4FB4-B0F7-CE2AC7157BE1}"/>
@@ -432,7 +432,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
       <c r="M1" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="RiV79UDehaDkj8Ifbx3VOBdPAwOFkI32t3/LVbTYrRsQrYijRwkZaM889Og7+1hOCfUtDZsKa4hBBBIuTPkyPw==" saltValue="q7PUUS1EfTvFDCV1LviGMw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="phc2gtloQpn7pLW9K3xy/Zr7qJLDmXaGc32OWAa2+1Wav1QfiFcC9DvUqvx+hhwyRteDMHjF5aYGdvTDfLNx4w==" saltValue="ZzI9h3zf/n9i1MLJ40o1PA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A1:J1" xr:uid="{F6B7ACFC-1D68-4C1C-85DA-B914FE1B0D40}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Read/Write features to SQLite connection
</commit_message>
<xml_diff>
--- a/Equipment_Registration_App/Equipment_Registration_App/Minuta_computadores.xlsx
+++ b/Equipment_Registration_App/Equipment_Registration_App/Minuta_computadores.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andresfelipe.perez\PycharmProjects\Equipment_Registration_App\Equipment_Registration_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429E190F-D113-47AE-912F-EAD482528061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8928846-D9D1-4A26-A4C8-C9DC573F916E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="148YiuHQ5lXJWUToTkvr1pwXzj+ON8cfZP+R9+O7wvSWExp7uaLSY8+ZU4BF1xL+EAgdMPlgOXlUkIOTH75cUA==" workbookSaltValue="r//egdUdAhMm1PxcbXxveQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-14460" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{25B8F748-A59F-4FB4-B0F7-CE2AC7157BE1}"/>
+    <workbookView xWindow="14340" yWindow="-16425" windowWidth="29040" windowHeight="15840" xr2:uid="{25B8F748-A59F-4FB4-B0F7-CE2AC7157BE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Minuta de registro" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Número serial</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>Información adicional</t>
+  </si>
+  <si>
+    <t>6WF2MN3</t>
+  </si>
+  <si>
+    <t>46243</t>
+  </si>
+  <si>
+    <t>Andrés Felipe Pérez</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5420</t>
+  </si>
+  <si>
+    <t>PC Laptop</t>
+  </si>
+  <si>
+    <t>Ingreso</t>
+  </si>
+  <si>
+    <t>ANDRESFELIPE.PEREZ</t>
   </si>
 </sst>
 </file>
@@ -428,11 +449,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B7ACFC-1D68-4C1C-85DA-B914FE1B0D40}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,8 +505,37 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45027.627129629633</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="phc2gtloQpn7pLW9K3xy/Zr7qJLDmXaGc32OWAa2+1Wav1QfiFcC9DvUqvx+hhwyRteDMHjF5aYGdvTDfLNx4w==" saltValue="ZzI9h3zf/n9i1MLJ40o1PA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="LmVSofdvJxxgCg98i0y5u8mSaKf64El6S9WCZwGcbt6yRfEwsECNuObYnQ4EUuGTIP8Ixp/qPjl4AeLdkQA+0Q==" saltValue="brSrbYPb45EKzaMVe+BPWg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A1:J1" xr:uid="{F6B7ACFC-1D68-4C1C-85DA-B914FE1B0D40}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>